<commit_message>
[!] Popisanie nejakych veci do Product Backlog.
Zatial nic takeho, co sa planuje este spravit.
</commit_message>
<xml_diff>
--- a/Dokumentacie/Ostatne/Product Backlog.xlsx
+++ b/Dokumentacie/Ostatne/Product Backlog.xlsx
@@ -16,33 +16,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Funkcionalita</t>
-  </si>
-  <si>
-    <t>Stav</t>
-  </si>
-  <si>
-    <t>Zaradenie podľa potreby</t>
-  </si>
-  <si>
-    <t>Musí byť</t>
-  </si>
-  <si>
-    <t>Mala by byť</t>
-  </si>
-  <si>
-    <t>Pekné keby bola</t>
-  </si>
-  <si>
-    <t>JADRO editora</t>
-  </si>
-  <si>
-    <t>Výhody</t>
-  </si>
-  <si>
-    <t>Používateľské rozhranie editora</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>CORE implementation</t>
+  </si>
+  <si>
+    <t>User Interface - GUI</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>must be</t>
+  </si>
+  <si>
+    <t>should be</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nice to have</t>
+  </si>
+  <si>
+    <t>Prirority</t>
+  </si>
+  <si>
+    <t>Dynamic work with AST tree with Lua</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>New type of grammar - ToDo list</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <t>Start page</t>
+  </si>
+  <si>
+    <t>Create new UI design</t>
+  </si>
+  <si>
+    <t>Bug report</t>
+  </si>
+  <si>
+    <t>New help on-line</t>
+  </si>
+  <si>
+    <t>About window</t>
+  </si>
+  <si>
+    <t>About this version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redesign menu bar and add new items </t>
+  </si>
+  <si>
+    <t>Fullscreen</t>
+  </si>
+  <si>
+    <t>New modern icons</t>
+  </si>
+  <si>
+    <t>Zoom in / out</t>
+  </si>
+  <si>
+    <t>Project tree</t>
+  </si>
+  <si>
+    <t>Bug list</t>
+  </si>
+  <si>
+    <t>Task list</t>
+  </si>
+  <si>
+    <t>Multitab editor</t>
+  </si>
+  <si>
+    <t>Shortcuts and actions defined with Lua</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>pouzit obr. pre status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallelism for full text analysis </t>
+  </si>
+  <si>
+    <t>Parallelism for blocks update</t>
+  </si>
+  <si>
+    <t>WORKING</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
   </si>
 </sst>
 </file>
@@ -168,13 +243,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,6 +257,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Kontrolná bunka" xfId="2" builtinId="23"/>
@@ -482,215 +562,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G22"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickTop="1">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.75" thickTop="1">
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="B17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="B18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="B19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="B20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="B22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="8"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
[!] Doplneny product backlog podla mojho odhadu.
Signed-off-by: xtursky <xtursky@gmail.com>
</commit_message>
<xml_diff>
--- a/Dokumentacie/Ostatne/Product Backlog.xlsx
+++ b/Dokumentacie/Ostatne/Product Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="21015" windowHeight="9690"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>Functionality</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Prirority</t>
   </si>
   <si>
-    <t>Dynamic work with AST tree with Lua</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>DONE</t>
   </si>
   <si>
-    <t>pouzit obr. pre status</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parallelism for full text analysis </t>
   </si>
   <si>
@@ -118,13 +112,55 @@
   </si>
   <si>
     <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Dynamic work with AST tree through Lua</t>
+  </si>
+  <si>
+    <t>Text operations (undo, redo, copy, paste)</t>
+  </si>
+  <si>
+    <t>Block operations (undo, redo)</t>
+  </si>
+  <si>
+    <t>INITIALIZED</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Ability to add user defined shortcuts and actions</t>
+  </si>
+  <si>
+    <t>Better code understanding</t>
+  </si>
+  <si>
+    <t>Faster content analyzing</t>
+  </si>
+  <si>
+    <t>Faster update of analyzed blocks</t>
+  </si>
+  <si>
+    <t>Faster and mainly non-blocking work</t>
+  </si>
+  <si>
+    <t>Simple and easy to view ToDo list with user tasks, which are fast to create and parsed by given grammar</t>
+  </si>
+  <si>
+    <t>Incorporate manipulation conventions into graphical mode of editor in the same way as for textual mode</t>
+  </si>
+  <si>
+    <t>Incorporate conventions with text manipulation as used from normal text editors</t>
+  </si>
+  <si>
+    <t>Newer and better looking UI for better visual experience</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +190,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -243,17 +287,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,24 +303,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Kontrolná bunka" xfId="2" builtinId="23"/>
-    <cellStyle name="normálne" xfId="0" builtinId="0"/>
-    <cellStyle name="Poznámka" xfId="3" builtinId="10"/>
-    <cellStyle name="Výstup" xfId="1" builtinId="21"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -352,6 +409,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -386,6 +444,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -561,17 +620,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -579,7 +638,7 @@
     <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -595,21 +654,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1">
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -618,110 +677,150 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="B4" s="6" t="s">
+      <c r="C6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="B5" s="6" t="s">
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="B8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="C10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
@@ -731,212 +830,255 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="6" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="6" t="s">
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="8"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="7"/>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="7"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -953,24 +1095,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[!] upraveny backlog a technicka dok. styly
</commit_message>
<xml_diff>
--- a/Dokumentacie/Ostatne/Product Backlog.xlsx
+++ b/Dokumentacie/Ostatne/Product Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="21015" windowHeight="9690"/>
@@ -159,8 +159,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,12 +296,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -317,12 +311,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
-    <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Kontrolná bunka" xfId="2" builtinId="23"/>
+    <cellStyle name="normálne" xfId="0" builtinId="0"/>
+    <cellStyle name="Poznámka" xfId="3" builtinId="10"/>
+    <cellStyle name="Výstup" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -335,7 +335,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -409,7 +409,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -444,7 +443,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -620,14 +618,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="39.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="52.85546875" style="1" customWidth="1"/>
@@ -638,25 +636,25 @@
     <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
@@ -666,418 +664,418 @@
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickTop="1">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="D4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="1:7">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:7">
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:7">
+      <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="D9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30">
+      <c r="B10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="D10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30">
+      <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+    <row r="12" spans="1:7">
+      <c r="B12" s="4"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="D14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:7">
+      <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="2:7">
+      <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="10" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+    <row r="26" spans="2:7">
+      <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="2:7">
+      <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="10" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
+    <row r="28" spans="2:7">
+      <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="5"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="5"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="2:7">
       <c r="B31" s="3"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="2:7">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2">
       <c r="B37" s="3"/>
     </row>
   </sheetData>
@@ -1095,24 +1093,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="49.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="13" max="14" width="8.28515625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>